<commit_message>
Adding local authority standardised rates over time to targets
</commit_message>
<xml_diff>
--- a/la_code_lookup.xlsx
+++ b/la_code_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/2025 projects/Describing NHP mitigators/nhp_community_mitigators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{449540D1-C2D5-46AF-8A9B-A77B7EFE683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{449540D1-C2D5-46AF-8A9B-A77B7EFE683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{599E63D1-E60D-43A6-92DE-A94C4CC4E7AA}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1944" windowWidth="20928" windowHeight="13800" xr2:uid="{247331CC-2092-4759-9157-6B10C70B4D05}"/>
+    <workbookView xWindow="8052" yWindow="1428" windowWidth="20928" windowHeight="13800" xr2:uid="{247331CC-2092-4759-9157-6B10C70B4D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>old_la_code</t>
   </si>
@@ -105,13 +105,79 @@
   </si>
   <si>
     <t>E06000064</t>
+  </si>
+  <si>
+    <t>E06000022</t>
+  </si>
+  <si>
+    <t>E06000023</t>
+  </si>
+  <si>
+    <t>E06000033</t>
+  </si>
+  <si>
+    <t>E07000004</t>
+  </si>
+  <si>
+    <t>E07000005</t>
+  </si>
+  <si>
+    <t>E07000006</t>
+  </si>
+  <si>
+    <t>E07000007</t>
+  </si>
+  <si>
+    <t>E07000076</t>
+  </si>
+  <si>
+    <t>E07000117</t>
+  </si>
+  <si>
+    <t>E07000150</t>
+  </si>
+  <si>
+    <t>E07000151</t>
+  </si>
+  <si>
+    <t>E07000152</t>
+  </si>
+  <si>
+    <t>E07000153</t>
+  </si>
+  <si>
+    <t>E07000154</t>
+  </si>
+  <si>
+    <t>E07000155</t>
+  </si>
+  <si>
+    <t>E07000156</t>
+  </si>
+  <si>
+    <t>E08000015</t>
+  </si>
+  <si>
+    <t>E08000032</t>
+  </si>
+  <si>
+    <t>E09000003</t>
+  </si>
+  <si>
+    <t>E06000060</t>
+  </si>
+  <si>
+    <t>E06000061</t>
+  </si>
+  <si>
+    <t>E06000062</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,30 +199,40 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF111111"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,30 +255,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -532,239 +629,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2778947-EB72-433E-97A4-9643F1954843}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="7" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding LA table and extending LA data to 2018/19
</commit_message>
<xml_diff>
--- a/la_code_lookup.xlsx
+++ b/la_code_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/2025 projects/Describing NHP mitigators/nhp_community_mitigators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{449540D1-C2D5-46AF-8A9B-A77B7EFE683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{599E63D1-E60D-43A6-92DE-A94C4CC4E7AA}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{449540D1-C2D5-46AF-8A9B-A77B7EFE683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C495401F-AD77-430B-BCC9-1F5E76E01842}"/>
   <bookViews>
-    <workbookView xWindow="8052" yWindow="1428" windowWidth="20928" windowHeight="13800" xr2:uid="{247331CC-2092-4759-9157-6B10C70B4D05}"/>
+    <workbookView xWindow="384" yWindow="0" windowWidth="8952" windowHeight="13800" xr2:uid="{247331CC-2092-4759-9157-6B10C70B4D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>old_la_code</t>
   </si>
@@ -171,13 +171,73 @@
   </si>
   <si>
     <t>E06000062</t>
+  </si>
+  <si>
+    <t>E06000028</t>
+  </si>
+  <si>
+    <t>E06000029</t>
+  </si>
+  <si>
+    <t>E06000037</t>
+  </si>
+  <si>
+    <t>E07000048</t>
+  </si>
+  <si>
+    <t>E07000049</t>
+  </si>
+  <si>
+    <t>E07000050</t>
+  </si>
+  <si>
+    <t>E07000051</t>
+  </si>
+  <si>
+    <t>E07000052</t>
+  </si>
+  <si>
+    <t>E07000053</t>
+  </si>
+  <si>
+    <t>E07000084</t>
+  </si>
+  <si>
+    <t>E07000190</t>
+  </si>
+  <si>
+    <t>E07000191</t>
+  </si>
+  <si>
+    <t>E07000201</t>
+  </si>
+  <si>
+    <t>E07000204</t>
+  </si>
+  <si>
+    <t>E07000205</t>
+  </si>
+  <si>
+    <t>E07000206</t>
+  </si>
+  <si>
+    <t>E06000058</t>
+  </si>
+  <si>
+    <t>E06000059</t>
+  </si>
+  <si>
+    <t>E07000245</t>
+  </si>
+  <si>
+    <t>E07000244</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,16 +294,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -251,11 +323,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,21 +357,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -629,17 +715,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2778947-EB72-433E-97A4-9643F1954843}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -650,7 +736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -659,7 +745,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -668,8 +754,9 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -678,8 +765,9 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -689,7 +777,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -699,7 +787,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -709,7 +797,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -728,7 +816,6 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -739,7 +826,6 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -750,7 +836,6 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -761,7 +846,6 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -772,7 +856,6 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -783,9 +866,8 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -795,7 +877,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -805,7 +887,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -815,7 +897,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -838,7 +920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
@@ -846,7 +928,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
@@ -854,13 +936,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -869,19 +952,19 @@
       <c r="B25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
@@ -890,7 +973,6 @@
       <c r="B28" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -899,7 +981,6 @@
       <c r="B29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
@@ -908,7 +989,6 @@
       <c r="B30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -917,7 +997,6 @@
       <c r="B31" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
@@ -926,46 +1005,165 @@
       <c r="B32" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A1:E4 A5:D23 A24:E37 A40:E40 A38:A39 C38:E39 A47:E47 A41:A46 C41:E46 A54:E1048576 A48:A53 C48:E53">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>